<commit_message>
MESI Test Cases added; test planning updated
</commit_message>
<xml_diff>
--- a/test_planning.xlsx
+++ b/test_planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MSI_Test" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="MESI_Test" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="130">
   <si>
     <t>Proc0</t>
   </si>
@@ -504,6 +505,533 @@
       </rPr>
       <t>, (M to I)</t>
     </r>
+  </si>
+  <si>
+    <t>Q1  LDR</t>
+  </si>
+  <si>
+    <t>PrWr/BusRd(S') CacheMiss,         (I to E)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrRd/BusRd(S')CacheMiss,       (I to E),       Wait bus queue until </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>101 cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>(E)                   0x7f0d3b28</t>
+  </si>
+  <si>
+    <t>Q4 STR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRdXCacheMiss,        (I to M),      Wait bus queue until </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>301 cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>Q5 LDR</t>
+  </si>
+  <si>
+    <t>(S) 0x7f0d3b30</t>
+  </si>
+  <si>
+    <t>(E) -&gt; (S) 0x7f0d3b30</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrRd/BusRd(S), CacheMiss,      at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycle 401</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when bus free, take 4 cycle to transfer from Proc1</t>
+    </r>
+  </si>
+  <si>
+    <t>CacheMiss,      (I to E),             (I to M)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycle 401</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see BusRd from Proc0, 2131573552    (E to S),       Flush to Mem</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRd(S)CacheMiss,        (I to S),               at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycle 405</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when bus free, take 4 cycle to transfer from Proc3</t>
+    </r>
+  </si>
+  <si>
+    <t>0x5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycle 405</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see BusRd from Proc2, 2131573568 (M to S), Flush to Mem</t>
+    </r>
+  </si>
+  <si>
+    <t>(M) -&gt; (S) 0x7f0d3b40</t>
+  </si>
+  <si>
+    <t>Q7 LDR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRd(S') CacheMiss,      (I to E),         Wait bus queue until  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>409 cycle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRdX CacheMiss,        (I to M),      Wait bus queue until </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>201 cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>(M) 0x7f0d3b40</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRdXCacheHit,        (S to M),      Wait bus queue until </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>509 cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>(S) -&gt; (I) 0x7f0d3b40</t>
+  </si>
+  <si>
+    <t>(M) -&gt; (I) 0x7f0d3b38</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>510 cycle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see BusRdX from Proc0, 2131573560 (M to I),         flush to mem</t>
+    </r>
+  </si>
+  <si>
+    <t>(E) 0x7f0d3b20</t>
+  </si>
+  <si>
+    <t>(E) -&gt; (I) 0x7f0d3b20</t>
+  </si>
+  <si>
+    <t>(S) 0x7f0d3b38</t>
+  </si>
+  <si>
+    <t>(M) -&gt; (S) 0x7f0d3b38</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRdX, CacheMiss, wait bus queue until </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>510 cycle,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> transfer from Proc2 cache with 4 cycle,     (I to M)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>509 cycle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see BusRdX from Proc3, 2131573568,    (S to I)</t>
+    </r>
+  </si>
+  <si>
+    <t>CacheMiss,      (I to S),              (E to S),           (M to S)</t>
+  </si>
+  <si>
+    <t>(M to S), CacheHit,         (E to E), CacheMiss,     (I to S),           (M to M)</t>
+  </si>
+  <si>
+    <t>(M) -&gt; (I) 0x7f0d3b40</t>
+  </si>
+  <si>
+    <t>PrRd/-, CacheHit,         (E to E),             no need wait bus</t>
+  </si>
+  <si>
+    <t>PrRd/-, CacheHit,      (M to M),       no need wait bus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRd(S), CacheMiss, wait bus queue until </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>514 cycle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, transfer from Proc0 cache with 4 cycle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>514 cycle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see BusRd from Proc2, 2131573560    (M to S)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrWr/BusRdX, CacheMiss, wait bus queue until </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>518 cycle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, transfer from Proc3 cache with 4 cycle,     (I to M)</t>
+    </r>
+  </si>
+  <si>
+    <t>0x8</t>
+  </si>
+  <si>
+    <t>CacheMiss,      (I to M),          (M to I)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycle 518</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see BusRdX from Proc0, 2131573568 (M to I),      flush to mem</t>
+    </r>
+  </si>
+  <si>
+    <t>Q14 STR</t>
+  </si>
+  <si>
+    <t>(M)  0x7f0d3b20</t>
+  </si>
+  <si>
+    <t>PrWr/BusRdX, CacheMiss, transfer from Proc1 with 4 cycles</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycle 522</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see busRdX from Proc2, 2131573536    (E to I),          flush to mem</t>
+    </r>
+  </si>
+  <si>
+    <t>(E to I), CacheMiss,      (I to M)</t>
+  </si>
+  <si>
+    <t>Q15 LDR</t>
+  </si>
+  <si>
+    <t>PrRd/-,     CacheHit,         no need bus</t>
+  </si>
+  <si>
+    <t>(E)  0x7f0d3b18</t>
+  </si>
+  <si>
+    <t>Q16 LDR</t>
+  </si>
+  <si>
+    <r>
+      <t>PrRd/BusRd(S')CacheMiss,       (I to E),            bus queue start at</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 522 cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>CacheHit,          (S to S), CacheMiss,      (I to E)</t>
+  </si>
+  <si>
+    <t>Q17 STR</t>
+  </si>
+  <si>
+    <t>(M)  0x7f0d3b18</t>
+  </si>
+  <si>
+    <t>PrWr/-, CacheHit,         no need bus</t>
+  </si>
+  <si>
+    <t>CacheHit,          (E to M)</t>
+  </si>
+  <si>
+    <t>Q18 STR</t>
+  </si>
+  <si>
+    <t>PrWr/-</t>
+  </si>
+  <si>
+    <t>CacheHit,        (M to M)</t>
+  </si>
+  <si>
+    <t>CacheMiss,       (I to M),            (M to I)</t>
+  </si>
+  <si>
+    <t>CacheMiss,      (I to E), CacheHit,             (S to I),               (S to M)</t>
   </si>
 </sst>
 </file>
@@ -562,7 +1090,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,8 +1133,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -673,11 +1207,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -747,9 +1325,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,6 +1333,63 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1075,9 +1707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1115,11 +1747,11 @@
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1129,11 +1761,11 @@
       <c r="G2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1143,11 +1775,11 @@
       <c r="M2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="38"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
       <c r="Q2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1157,11 +1789,11 @@
       <c r="S2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="T2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="37"/>
-      <c r="V2" s="38"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="37"/>
       <c r="W2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1642,7 +2274,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -1718,7 +2350,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
@@ -1789,7 +2421,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="16" t="s">
         <v>20</v>
       </c>
@@ -1942,7 +2574,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="38" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -2021,7 +2653,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="16" t="s">
         <v>20</v>
       </c>
@@ -2110,6 +2742,975 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="14" customWidth="1"/>
+    <col min="6" max="7" width="5.140625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" style="16" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="14" customWidth="1"/>
+    <col min="12" max="13" width="5.140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" style="16" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="11" style="10" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="14" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" style="17" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" style="16" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11" style="10" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="14" customWidth="1"/>
+    <col min="24" max="25" width="5.140625" style="17" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="36"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="23">
+        <v>2131573544</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="25">
+        <v>1</v>
+      </c>
+      <c r="G3" s="25">
+        <f>F3+99</f>
+        <v>100</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="26">
+        <v>2131573552</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="25">
+        <v>1</v>
+      </c>
+      <c r="M3" s="25">
+        <f>L3+199</f>
+        <v>200</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="P3" s="12">
+        <v>2131573560</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="R3" s="25">
+        <v>1</v>
+      </c>
+      <c r="S3" s="25">
+        <f>R3+299</f>
+        <v>300</v>
+      </c>
+      <c r="T3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="V3" s="27">
+        <v>2131573568</v>
+      </c>
+      <c r="W3" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="X3" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="25">
+        <f>X3+399</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10">
+        <v>4</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30">
+        <f t="shared" ref="F4" si="0">G3+1</f>
+        <v>101</v>
+      </c>
+      <c r="G4" s="30">
+        <f>F4+3</f>
+        <v>104</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="10">
+        <v>4</v>
+      </c>
+      <c r="L4" s="17">
+        <f t="shared" ref="L4" si="1">M3+1</f>
+        <v>201</v>
+      </c>
+      <c r="M4" s="17">
+        <f>L4+3</f>
+        <v>204</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="10">
+        <v>4</v>
+      </c>
+      <c r="R4" s="17">
+        <f t="shared" ref="R4" si="2">S3+1</f>
+        <v>301</v>
+      </c>
+      <c r="S4" s="17">
+        <f>R4+3</f>
+        <v>304</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" s="10">
+        <v>3</v>
+      </c>
+      <c r="X4" s="17">
+        <f t="shared" ref="X4" si="3">Y3+1</f>
+        <v>401</v>
+      </c>
+      <c r="Y4" s="17">
+        <f>X4+2</f>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="26">
+        <v>2131573552</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="17">
+        <f>G4+1</f>
+        <v>105</v>
+      </c>
+      <c r="G5" s="17">
+        <f>Y3+4</f>
+        <v>404</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="10">
+        <v>200</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="17">
+        <f>M4+1</f>
+        <v>205</v>
+      </c>
+      <c r="M5" s="17">
+        <f>G5</f>
+        <v>404</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="P5" s="27">
+        <v>2131573568</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="17">
+        <f>S4+1</f>
+        <v>305</v>
+      </c>
+      <c r="S5" s="17">
+        <f>G5+4</f>
+        <v>408</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="V5" s="10">
+        <v>5</v>
+      </c>
+      <c r="W5" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="X5" s="17">
+        <f>Y4+1</f>
+        <v>404</v>
+      </c>
+      <c r="Y5" s="17">
+        <f>X5+4</f>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="10">
+        <v>4</v>
+      </c>
+      <c r="F6" s="17">
+        <f>G5+1</f>
+        <v>405</v>
+      </c>
+      <c r="G6" s="17">
+        <f>F6+3</f>
+        <v>408</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="13">
+        <v>2131573536</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="17">
+        <f>M5+1</f>
+        <v>405</v>
+      </c>
+      <c r="M6" s="17">
+        <f>S5+100</f>
+        <v>508</v>
+      </c>
+      <c r="N6" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" s="44">
+        <v>104</v>
+      </c>
+      <c r="Q6" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="R6" s="46">
+        <f>S5+1</f>
+        <v>409</v>
+      </c>
+      <c r="S6" s="46">
+        <f>R6+103</f>
+        <v>512</v>
+      </c>
+      <c r="T6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="V6" s="27">
+        <v>2131573568</v>
+      </c>
+      <c r="W6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="X6" s="17">
+        <f>Y5+1</f>
+        <v>409</v>
+      </c>
+      <c r="Y6" s="17">
+        <f>M6+1</f>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="12">
+        <v>2131573560</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="17">
+        <f>G6+1</f>
+        <v>409</v>
+      </c>
+      <c r="G7" s="17">
+        <f>Y6+4</f>
+        <v>513</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="10">
+        <v>4</v>
+      </c>
+      <c r="L7" s="17">
+        <f>M6+1</f>
+        <v>509</v>
+      </c>
+      <c r="M7" s="17">
+        <f>L7+3</f>
+        <v>512</v>
+      </c>
+      <c r="N7" s="38"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="V7" s="10">
+        <v>2</v>
+      </c>
+      <c r="X7" s="17">
+        <f>Y6+1</f>
+        <v>510</v>
+      </c>
+      <c r="Y7" s="17">
+        <f>X7+1</f>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="17">
+        <f>G7+1</f>
+        <v>514</v>
+      </c>
+      <c r="G8" s="17">
+        <f>F8+1</f>
+        <v>515</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="13">
+        <v>2131573536</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" s="17">
+        <f>M7+1</f>
+        <v>513</v>
+      </c>
+      <c r="M8" s="17">
+        <f>L8</f>
+        <v>513</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="P8" s="12">
+        <v>2131573560</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="R8" s="17">
+        <f>S6+1</f>
+        <v>513</v>
+      </c>
+      <c r="S8" s="17">
+        <f>R8+4</f>
+        <v>517</v>
+      </c>
+      <c r="T8" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="V8" s="27">
+        <v>2131573568</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="X8" s="17">
+        <f>Y7+1</f>
+        <v>512</v>
+      </c>
+      <c r="Y8" s="17">
+        <f>X8</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="27">
+        <v>2131573568</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="17">
+        <f>G8+1</f>
+        <v>516</v>
+      </c>
+      <c r="G9" s="17">
+        <f>F9+5</f>
+        <v>521</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="10">
+        <v>4</v>
+      </c>
+      <c r="L9" s="17">
+        <f>M8+1</f>
+        <v>514</v>
+      </c>
+      <c r="M9" s="17">
+        <f>L9+3</f>
+        <v>517</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="10">
+        <v>4</v>
+      </c>
+      <c r="R9" s="17">
+        <f>S8+1</f>
+        <v>518</v>
+      </c>
+      <c r="S9" s="17">
+        <f>R9+3</f>
+        <v>521</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="V9" s="10">
+        <v>8</v>
+      </c>
+      <c r="W9" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="X9" s="17">
+        <f>Y8+1</f>
+        <v>513</v>
+      </c>
+      <c r="Y9" s="17">
+        <f>X9+7</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="17">
+        <f>G9+1</f>
+        <v>522</v>
+      </c>
+      <c r="G10" s="17">
+        <f>F10+3</f>
+        <v>525</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="10">
+        <v>4</v>
+      </c>
+      <c r="L10" s="17">
+        <f>M9+1</f>
+        <v>518</v>
+      </c>
+      <c r="M10" s="17">
+        <f>L10+3</f>
+        <v>521</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="O10" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="P10" s="13">
+        <v>2131573536</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="R10" s="17">
+        <f>S9+1</f>
+        <v>522</v>
+      </c>
+      <c r="S10" s="17">
+        <f>R10+3</f>
+        <v>525</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="V10" s="10">
+        <v>4</v>
+      </c>
+      <c r="X10" s="17">
+        <f>Y9+1</f>
+        <v>521</v>
+      </c>
+      <c r="Y10" s="17">
+        <f>X10+3</f>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="26">
+        <v>2131573552</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="17">
+        <f>G10+1</f>
+        <v>526</v>
+      </c>
+      <c r="G11" s="17">
+        <f>F11</f>
+        <v>526</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="48">
+        <v>2131573528</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="L11" s="55">
+        <v>522</v>
+      </c>
+      <c r="M11" s="55">
+        <f>L11+99</f>
+        <v>621</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="10">
+        <v>4</v>
+      </c>
+      <c r="R11" s="17">
+        <f>S10+1</f>
+        <v>526</v>
+      </c>
+      <c r="S11" s="17">
+        <f>R11+3</f>
+        <v>529</v>
+      </c>
+      <c r="T11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="V11" s="10">
+        <v>4</v>
+      </c>
+      <c r="X11" s="17">
+        <f>Y10+1</f>
+        <v>525</v>
+      </c>
+      <c r="Y11" s="17">
+        <f>X11+3</f>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="10">
+        <v>4</v>
+      </c>
+      <c r="F12" s="17">
+        <f>G11+1</f>
+        <v>527</v>
+      </c>
+      <c r="G12" s="17">
+        <f>F12+3</f>
+        <v>530</v>
+      </c>
+      <c r="H12" s="50"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+    </row>
+    <row r="13" spans="1:25" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="52">
+        <v>4</v>
+      </c>
+      <c r="L13" s="56">
+        <f>M11+1</f>
+        <v>622</v>
+      </c>
+      <c r="M13" s="56">
+        <f>L13+3</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="48">
+        <v>2131573528</v>
+      </c>
+      <c r="K14" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="L14" s="55">
+        <f>M13+1</f>
+        <v>626</v>
+      </c>
+      <c r="M14" s="55">
+        <f>L14</f>
+        <v>626</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+    </row>
+    <row r="16" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="52">
+        <v>4</v>
+      </c>
+      <c r="L16" s="17">
+        <f>M14+1</f>
+        <v>627</v>
+      </c>
+      <c r="M16" s="17">
+        <f>L16+3</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="J17" s="48">
+        <v>2131573528</v>
+      </c>
+      <c r="K17" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="L17" s="17">
+        <f>M16+1</f>
+        <v>631</v>
+      </c>
+      <c r="M17" s="17">
+        <f>L17</f>
+        <v>631</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="50"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="T2:V2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
More Dragon bugfixes. Final test case edits.
</commit_message>
<xml_diff>
--- a/test_planning.xlsx
+++ b/test_planning.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Desktop\Chowder Backup\Eric NUS\Year 4\Sem1\CS4223 Multi-core Architectures\Assignments\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7500"/>
+    <workbookView xWindow="29580" yWindow="0" windowWidth="26120" windowHeight="18680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MSI_Test" sheetId="1" r:id="rId1"/>
     <sheet name="MESI_Test" sheetId="4" r:id="rId2"/>
     <sheet name="DRAGON_Test" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -2160,7 +2158,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2264,16 +2262,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2282,7 +2280,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2290,33 +2288,33 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -2325,7 +2323,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -2334,34 +2332,34 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2475,27 +2473,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2507,6 +2484,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2568,7 +2566,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2620,7 +2618,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2814,7 +2812,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2824,43 +2822,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="7" customWidth="1"/>
-    <col min="6" max="7" width="5.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="7" customWidth="1"/>
-    <col min="12" max="13" width="5.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="7" customWidth="1"/>
+    <col min="6" max="7" width="5.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" style="7" customWidth="1"/>
+    <col min="12" max="13" width="5.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="7" customWidth="1"/>
-    <col min="18" max="19" width="5.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" style="7" customWidth="1"/>
+    <col min="18" max="19" width="5.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="5.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="3"/>
+    <col min="23" max="23" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="5.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="29" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -2921,7 +2919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="99" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
@@ -3002,7 +3000,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="70.5" customHeight="1" thickBot="1">
       <c r="A4" s="21"/>
       <c r="B4" s="9" t="s">
         <v>10</v>
@@ -3074,7 +3072,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="71" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -3152,7 +3150,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="115.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="113" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -3230,7 +3228,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="85" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
@@ -3307,7 +3305,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="99" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
@@ -3385,7 +3383,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="43" thickBot="1">
       <c r="A9" s="44" t="s">
         <v>19</v>
       </c>
@@ -3461,7 +3459,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15" thickBot="1">
       <c r="A10" s="44"/>
       <c r="B10" s="9" t="s">
         <v>10</v>
@@ -3532,7 +3530,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="29" thickBot="1">
       <c r="A11" s="44"/>
       <c r="B11" s="9" t="s">
         <v>10</v>
@@ -3606,7 +3604,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="85" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
@@ -3684,7 +3682,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="99" thickBot="1">
       <c r="A13" s="44" t="s">
         <v>22</v>
       </c>
@@ -3762,7 +3760,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="84">
       <c r="A14" s="44"/>
       <c r="B14" s="9" t="s">
         <v>10</v>
@@ -3836,7 +3834,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22">
       <c r="A17" s="9" t="s">
         <v>92</v>
       </c>
@@ -3862,7 +3860,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="28">
       <c r="A18" s="9" t="s">
         <v>93</v>
       </c>
@@ -3873,13 +3871,13 @@
         <v>93</v>
       </c>
       <c r="J18" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O18" s="9" t="s">
         <v>93</v>
       </c>
       <c r="P18" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U18" s="9" t="s">
         <v>93</v>
@@ -3888,7 +3886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="28">
       <c r="A19" s="9" t="s">
         <v>94</v>
       </c>
@@ -3899,13 +3897,13 @@
         <v>94</v>
       </c>
       <c r="J19" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O19" s="9" t="s">
         <v>94</v>
       </c>
       <c r="P19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U19" s="9" t="s">
         <v>94</v>
@@ -3914,7 +3912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22">
       <c r="A20" s="9" t="s">
         <v>95</v>
       </c>
@@ -3940,7 +3938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22">
       <c r="A21" s="9" t="s">
         <v>96</v>
       </c>
@@ -3966,7 +3964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22">
       <c r="A22" s="9" t="s">
         <v>97</v>
       </c>
@@ -3992,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22">
       <c r="A23" s="9" t="s">
         <v>98</v>
       </c>
@@ -4003,13 +4001,13 @@
         <v>98</v>
       </c>
       <c r="J23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O23" s="9" t="s">
         <v>98</v>
       </c>
       <c r="P23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U23" s="9" t="s">
         <v>98</v>
@@ -4028,7 +4026,11 @@
     <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4036,43 +4038,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="7" customWidth="1"/>
-    <col min="6" max="7" width="5.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="7" customWidth="1"/>
-    <col min="12" max="13" width="5.140625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="9" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="7" customWidth="1"/>
+    <col min="6" max="7" width="5.1640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="7" customWidth="1"/>
+    <col min="12" max="13" width="5.1640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="4.5" style="9" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="3" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="7" customWidth="1"/>
-    <col min="18" max="19" width="5.140625" style="10" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" style="9" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="7" customWidth="1"/>
+    <col min="18" max="19" width="5.1640625" style="10" customWidth="1"/>
+    <col min="20" max="20" width="4.5" style="9" customWidth="1"/>
+    <col min="21" max="21" width="10.5" style="3" customWidth="1"/>
     <col min="22" max="22" width="11" style="3" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" style="7" customWidth="1"/>
-    <col min="24" max="25" width="5.140625" style="10" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="3"/>
+    <col min="23" max="23" width="11.83203125" style="7" customWidth="1"/>
+    <col min="24" max="25" width="5.1640625" style="10" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="29" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -4133,7 +4135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="99" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>49</v>
       </c>
@@ -4214,7 +4216,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="70.5" customHeight="1" thickBot="1">
       <c r="A4" s="21"/>
       <c r="B4" s="9" t="s">
         <v>10</v>
@@ -4286,7 +4288,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="99" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>65</v>
       </c>
@@ -4371,7 +4373,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="85" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>91</v>
       </c>
@@ -4412,23 +4414,23 @@
         <f>S5+100</f>
         <v>508</v>
       </c>
-      <c r="N6" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="53" t="s">
+      <c r="N6" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="P6" s="53">
+      <c r="P6" s="46">
         <v>104</v>
       </c>
       <c r="Q6" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="55">
+      <c r="R6" s="48">
         <f>S5+1</f>
         <v>409</v>
       </c>
-      <c r="S6" s="55">
+      <c r="S6" s="48">
         <f>R6+103</f>
         <v>512</v>
       </c>
@@ -4453,7 +4455,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="99" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>90</v>
       </c>
@@ -4495,13 +4497,13 @@
         <v>512</v>
       </c>
       <c r="N7" s="44"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
       <c r="Q7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="R7" s="55"/>
-      <c r="S7" s="55"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
       <c r="T7" s="9" t="s">
         <v>10</v>
       </c>
@@ -4520,7 +4522,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="99" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>66</v>
       </c>
@@ -4605,7 +4607,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="99" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>74</v>
       </c>
@@ -4684,7 +4686,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="71" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>78</v>
       </c>
@@ -4760,7 +4762,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="77.25" customHeight="1" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>83</v>
       </c>
@@ -4787,19 +4789,19 @@
       <c r="H11" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="48">
+      <c r="J11" s="52">
         <v>2131573528</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="L11" s="45">
+      <c r="L11" s="53">
         <v>522</v>
       </c>
-      <c r="M11" s="45">
+      <c r="M11" s="53">
         <f>L11+99</f>
         <v>621</v>
       </c>
@@ -4838,7 +4840,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="76.5" customHeight="1" thickBot="1">
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
@@ -4857,15 +4859,15 @@
         <v>530</v>
       </c>
       <c r="H12" s="50"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="48"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="52"/>
       <c r="K12" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-    </row>
-    <row r="13" spans="1:25" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+    </row>
+    <row r="13" spans="1:25" ht="76.5" customHeight="1" thickBot="1">
       <c r="H13" s="32" t="s">
         <v>10</v>
       </c>
@@ -4884,41 +4886,41 @@
         <v>625</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+    <row r="14" spans="1:25" ht="26.25" customHeight="1">
+      <c r="A14" s="54" t="s">
         <v>87</v>
       </c>
       <c r="H14" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="48">
+      <c r="J14" s="52">
         <v>2131573528</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="45">
+      <c r="L14" s="53">
         <f>M13+1</f>
         <v>626</v>
       </c>
-      <c r="M14" s="45">
+      <c r="M14" s="53">
         <f>L14</f>
         <v>626</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
+    <row r="15" spans="1:25" ht="15" thickBot="1">
+      <c r="A15" s="54"/>
       <c r="H15" s="50"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-    </row>
-    <row r="16" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+    </row>
+    <row r="16" spans="1:25" ht="15" thickBot="1">
       <c r="H16" s="32" t="s">
         <v>10</v>
       </c>
@@ -4937,20 +4939,20 @@
         <v>630</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="25.5" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>89</v>
       </c>
       <c r="H17" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="47" t="s">
+      <c r="I17" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="J17" s="48">
+      <c r="J17" s="52">
         <v>2131573528</v>
       </c>
-      <c r="K17" s="51" t="s">
+      <c r="K17" s="55" t="s">
         <v>86</v>
       </c>
       <c r="L17" s="10">
@@ -4962,13 +4964,13 @@
         <v>631</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15" thickBot="1">
       <c r="H18" s="50"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="51"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="55"/>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="9" t="s">
         <v>92</v>
       </c>
@@ -4994,7 +4996,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" ht="28">
       <c r="A21" s="9" t="s">
         <v>93</v>
       </c>
@@ -5020,7 +5022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" ht="28">
       <c r="A22" s="9" t="s">
         <v>94</v>
       </c>
@@ -5046,7 +5048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22">
       <c r="A23" s="9" t="s">
         <v>95</v>
       </c>
@@ -5072,7 +5074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -5098,7 +5100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22">
       <c r="A25" s="9" t="s">
         <v>97</v>
       </c>
@@ -5124,7 +5126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -5152,20 +5154,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
     <mergeCell ref="M14:M15"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="I17:I18"/>
@@ -5177,9 +5165,27 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5192,38 +5198,38 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="7" customWidth="1"/>
-    <col min="6" max="7" width="5.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="7" customWidth="1"/>
-    <col min="12" max="13" width="5.140625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="9" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="7" customWidth="1"/>
+    <col min="6" max="7" width="5.1640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="7" customWidth="1"/>
+    <col min="12" max="13" width="5.1640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="4.5" style="9" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="3" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.85546875" style="7" customWidth="1"/>
-    <col min="18" max="19" width="5.140625" style="10" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" style="9" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" style="7" customWidth="1"/>
+    <col min="18" max="19" width="5.1640625" style="10" customWidth="1"/>
+    <col min="20" max="20" width="4.5" style="9" customWidth="1"/>
+    <col min="21" max="21" width="10.5" style="3" customWidth="1"/>
     <col min="22" max="22" width="11" style="3" customWidth="1"/>
     <col min="23" max="23" width="17" style="7" customWidth="1"/>
-    <col min="24" max="25" width="5.140625" style="10" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="3"/>
+    <col min="24" max="25" width="5.1640625" style="10" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="29" thickBot="1">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -5284,7 +5290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="71" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>146</v>
       </c>
@@ -5365,7 +5371,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15" thickBot="1">
       <c r="A4" s="21"/>
       <c r="B4" s="9" t="s">
         <v>10</v>
@@ -5437,7 +5443,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="71" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>148</v>
       </c>
@@ -5522,7 +5528,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="71" thickBot="1">
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
@@ -5595,7 +5601,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="99" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>165</v>
       </c>
@@ -5675,7 +5681,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="43" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>159</v>
       </c>
@@ -5754,7 +5760,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="71" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>163</v>
       </c>
@@ -5830,7 +5836,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="71" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>169</v>
       </c>
@@ -5909,7 +5915,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="71" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>171</v>
       </c>
@@ -5988,7 +5994,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="85" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>180</v>
       </c>
@@ -6069,7 +6075,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" ht="112">
       <c r="A13" s="9" t="s">
         <v>182</v>
       </c>
@@ -6128,12 +6134,12 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25">
       <c r="N14" s="21"/>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
     </row>
-    <row r="17" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" s="7" customFormat="1">
       <c r="A17" s="9" t="s">
         <v>92</v>
       </c>
@@ -6172,7 +6178,7 @@
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="1:25" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" s="7" customFormat="1" ht="28">
       <c r="A18" s="9" t="s">
         <v>93</v>
       </c>
@@ -6211,7 +6217,7 @@
       <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
     </row>
-    <row r="19" spans="1:25" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" s="7" customFormat="1" ht="28">
       <c r="A19" s="9" t="s">
         <v>94</v>
       </c>
@@ -6250,7 +6256,7 @@
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
     </row>
-    <row r="20" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" s="7" customFormat="1">
       <c r="A20" s="9" t="s">
         <v>95</v>
       </c>
@@ -6289,7 +6295,7 @@
       <c r="X20" s="10"/>
       <c r="Y20" s="10"/>
     </row>
-    <row r="21" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" s="7" customFormat="1">
       <c r="A21" s="9" t="s">
         <v>96</v>
       </c>
@@ -6328,7 +6334,7 @@
       <c r="X21" s="10"/>
       <c r="Y21" s="10"/>
     </row>
-    <row r="22" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" s="7" customFormat="1">
       <c r="A22" s="9" t="s">
         <v>97</v>
       </c>
@@ -6367,7 +6373,7 @@
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
     </row>
-    <row r="23" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" s="7" customFormat="1">
       <c r="A23" s="9" t="s">
         <v>98</v>
       </c>
@@ -6406,7 +6412,7 @@
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25">
       <c r="B24" s="38"/>
     </row>
   </sheetData>
@@ -6417,6 +6423,10 @@
     <mergeCell ref="T2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>